<commit_message>
Finished checking all links by hand
</commit_message>
<xml_diff>
--- a/analysis_2023-05/linksToCheck.xlsx
+++ b/analysis_2023-05/linksToCheck.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="4-linksToCheck" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="702">
   <si>
     <t>eprint_id</t>
   </si>
@@ -2074,6 +2074,57 @@
   </si>
   <si>
     <t>https://figshare.com/articles/dataset/A_Multi-Year_Data_Set_on_Aerosol-Cloud-Precipitation-Meteorology_Interactions_for_Marine_Stratocumulus_Clouds/5099983</t>
+  </si>
+  <si>
+    <t>error in DOI, resolves to homepage</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.7909/C3WD3xH1</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>Supplemental material</t>
+  </si>
+  <si>
+    <t>https://search.earthdata.nasa.gov/search/granules?p=C1288777617-LARC</t>
+  </si>
+  <si>
+    <t>https://www.bgc-jena.mpg.de/bgi/index.php/Services/Overview</t>
+  </si>
+  <si>
+    <t>Record removed from zenodo, marked as 'spam record'</t>
+  </si>
+  <si>
+    <t>doi.org message</t>
+  </si>
+  <si>
+    <t>site not responding</t>
+  </si>
+  <si>
+    <t>figshare page not found</t>
+  </si>
+  <si>
+    <t>Weird error message (not from doi.org)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.821582</t>
+  </si>
+  <si>
+    <t>https://figshare.com/projects/Tabula_Muris_Transcriptomic_characterization_of_20_organs_and_tissues_from_Mus_musculus_at_single_cell_resolution/27733</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/sambrooke/avulsionflood-scour-paper/-/releases/v1.2</t>
+  </si>
+  <si>
+    <t>Routes to make an account screen</t>
+  </si>
+  <si>
+    <t>Data repository moved to figshare</t>
+  </si>
+  <si>
+    <t>connection not private warning</t>
   </si>
 </sst>
 </file>
@@ -2896,9 +2947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P233" sqref="P233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3005,8 +3056,8 @@
       <c r="O2">
         <v>404</v>
       </c>
-      <c r="P2" t="b">
-        <v>1</v>
+      <c r="P2" t="s">
+        <v>687</v>
       </c>
       <c r="Q2" t="s">
         <v>672</v>
@@ -4023,8 +4074,8 @@
       <c r="O22">
         <v>404</v>
       </c>
-      <c r="P22" t="b">
-        <v>1</v>
+      <c r="P22" t="s">
+        <v>687</v>
       </c>
       <c r="Q22" t="s">
         <v>672</v>
@@ -5212,8 +5263,8 @@
       <c r="O45">
         <v>404</v>
       </c>
-      <c r="P45" t="b">
-        <v>1</v>
+      <c r="P45" t="s">
+        <v>687</v>
       </c>
       <c r="Q45" t="s">
         <v>672</v>
@@ -5518,8 +5569,8 @@
       <c r="O51">
         <v>404</v>
       </c>
-      <c r="P51" t="b">
-        <v>1</v>
+      <c r="P51" t="s">
+        <v>687</v>
       </c>
       <c r="Q51" t="s">
         <v>672</v>
@@ -5559,7 +5610,7 @@
       <c r="J52" t="s">
         <v>20</v>
       </c>
-      <c r="K52" t="s">
+      <c r="K52" s="4" t="s">
         <v>156</v>
       </c>
       <c r="L52" t="s">
@@ -5573,6 +5624,9 @@
       </c>
       <c r="O52">
         <v>404</v>
+      </c>
+      <c r="P52" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
@@ -5606,7 +5660,7 @@
       <c r="J53" t="s">
         <v>20</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K53" s="4" t="s">
         <v>157</v>
       </c>
       <c r="L53" t="s">
@@ -5620,6 +5674,9 @@
       </c>
       <c r="O53">
         <v>404</v>
+      </c>
+      <c r="P53" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
@@ -5653,7 +5710,7 @@
       <c r="J54" t="s">
         <v>162</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K54" s="4" t="s">
         <v>159</v>
       </c>
       <c r="L54" t="s">
@@ -5667,6 +5724,15 @@
       </c>
       <c r="O54">
         <v>404</v>
+      </c>
+      <c r="P54" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>685</v>
+      </c>
+      <c r="R54" s="4" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
@@ -5700,7 +5766,7 @@
       <c r="J55" t="s">
         <v>20</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K55" s="4" t="s">
         <v>164</v>
       </c>
       <c r="L55" t="s">
@@ -5714,6 +5780,9 @@
       </c>
       <c r="O55">
         <v>404</v>
+      </c>
+      <c r="P55" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
@@ -5747,7 +5816,7 @@
       <c r="J56" t="s">
         <v>20</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K56" s="4" t="s">
         <v>167</v>
       </c>
       <c r="L56" t="s">
@@ -5761,6 +5830,12 @@
       </c>
       <c r="O56">
         <v>404</v>
+      </c>
+      <c r="P56" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
@@ -5794,7 +5869,7 @@
       <c r="J57" t="s">
         <v>20</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K57" s="4" t="s">
         <v>170</v>
       </c>
       <c r="L57" t="s">
@@ -5808,6 +5883,12 @@
       </c>
       <c r="O57">
         <v>404</v>
+      </c>
+      <c r="P57" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
@@ -5841,7 +5922,7 @@
       <c r="J58" t="s">
         <v>20</v>
       </c>
-      <c r="K58" t="s">
+      <c r="K58" s="4" t="s">
         <v>173</v>
       </c>
       <c r="L58" t="s">
@@ -5855,6 +5936,9 @@
       </c>
       <c r="O58">
         <v>404</v>
+      </c>
+      <c r="P58" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
@@ -5888,7 +5972,7 @@
       <c r="J59" t="s">
         <v>20</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K59" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L59" t="s">
@@ -5902,6 +5986,12 @@
       </c>
       <c r="O59">
         <v>404</v>
+      </c>
+      <c r="P59" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
@@ -5935,7 +6025,7 @@
       <c r="J60" t="s">
         <v>20</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K60" s="4" t="s">
         <v>177</v>
       </c>
       <c r="L60" t="s">
@@ -5949,6 +6039,9 @@
       </c>
       <c r="O60">
         <v>404</v>
+      </c>
+      <c r="P60" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
@@ -5982,7 +6075,7 @@
       <c r="J61" t="s">
         <v>20</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K61" s="4" t="s">
         <v>179</v>
       </c>
       <c r="L61" t="s">
@@ -5996,6 +6089,9 @@
       </c>
       <c r="O61">
         <v>404</v>
+      </c>
+      <c r="P61" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
@@ -6029,7 +6125,7 @@
       <c r="J62" t="s">
         <v>20</v>
       </c>
-      <c r="K62" t="s">
+      <c r="K62" s="4" t="s">
         <v>181</v>
       </c>
       <c r="L62" t="s">
@@ -6043,6 +6139,9 @@
       </c>
       <c r="O62">
         <v>404</v>
+      </c>
+      <c r="P62" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
@@ -6076,7 +6175,7 @@
       <c r="J63" t="s">
         <v>20</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K63" s="4" t="s">
         <v>183</v>
       </c>
       <c r="L63" t="s">
@@ -6090,6 +6189,9 @@
       </c>
       <c r="O63">
         <v>404</v>
+      </c>
+      <c r="P63" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
@@ -6123,7 +6225,7 @@
       <c r="J64" t="s">
         <v>20</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K64" s="4" t="s">
         <v>184</v>
       </c>
       <c r="L64" t="s">
@@ -6138,8 +6240,11 @@
       <c r="O64">
         <v>404</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>72509</v>
       </c>
@@ -6170,7 +6275,7 @@
       <c r="J65" t="s">
         <v>20</v>
       </c>
-      <c r="K65" t="s">
+      <c r="K65" s="4" t="s">
         <v>185</v>
       </c>
       <c r="L65" t="s">
@@ -6185,8 +6290,11 @@
       <c r="O65">
         <v>404</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>72179</v>
       </c>
@@ -6217,7 +6325,7 @@
       <c r="J66" t="s">
         <v>20</v>
       </c>
-      <c r="K66" t="s">
+      <c r="K66" s="4" t="s">
         <v>187</v>
       </c>
       <c r="L66" t="s">
@@ -6232,8 +6340,11 @@
       <c r="O66">
         <v>404</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>70618</v>
       </c>
@@ -6264,7 +6375,7 @@
       <c r="J67" t="s">
         <v>20</v>
       </c>
-      <c r="K67" t="s">
+      <c r="K67" s="4" t="s">
         <v>191</v>
       </c>
       <c r="L67" t="s">
@@ -6279,8 +6390,14 @@
       <c r="O67">
         <v>404</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P67" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>69816</v>
       </c>
@@ -6311,7 +6428,7 @@
       <c r="J68" t="s">
         <v>20</v>
       </c>
-      <c r="K68" t="s">
+      <c r="K68" s="4" t="s">
         <v>194</v>
       </c>
       <c r="L68" t="s">
@@ -6326,8 +6443,11 @@
       <c r="O68">
         <v>404</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>69795</v>
       </c>
@@ -6358,7 +6478,7 @@
       <c r="J69" t="s">
         <v>20</v>
       </c>
-      <c r="K69" t="s">
+      <c r="K69" s="4" t="s">
         <v>197</v>
       </c>
       <c r="L69" t="s">
@@ -6373,8 +6493,14 @@
       <c r="O69">
         <v>404</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P69" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69094</v>
       </c>
@@ -6405,7 +6531,7 @@
       <c r="J70" t="s">
         <v>20</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K70" s="4" t="s">
         <v>199</v>
       </c>
       <c r="L70" t="s">
@@ -6420,8 +6546,14 @@
       <c r="O70">
         <v>404</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P70" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>67865</v>
       </c>
@@ -6452,7 +6584,7 @@
       <c r="J71" t="s">
         <v>20</v>
       </c>
-      <c r="K71" t="s">
+      <c r="K71" s="4" t="s">
         <v>202</v>
       </c>
       <c r="L71" t="s">
@@ -6467,8 +6599,11 @@
       <c r="O71">
         <v>404</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>67366</v>
       </c>
@@ -6499,7 +6634,7 @@
       <c r="J72" t="s">
         <v>20</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K72" s="4" t="s">
         <v>206</v>
       </c>
       <c r="L72" t="s">
@@ -6514,8 +6649,11 @@
       <c r="O72">
         <v>404</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>66233</v>
       </c>
@@ -6546,7 +6684,7 @@
       <c r="J73" t="s">
         <v>20</v>
       </c>
-      <c r="K73" t="s">
+      <c r="K73" s="4" t="s">
         <v>208</v>
       </c>
       <c r="L73" t="s">
@@ -6561,8 +6699,11 @@
       <c r="O73">
         <v>404</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>62464</v>
       </c>
@@ -6593,7 +6734,7 @@
       <c r="J74" t="s">
         <v>20</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K74" s="4" t="s">
         <v>212</v>
       </c>
       <c r="L74" t="s">
@@ -6608,8 +6749,14 @@
       <c r="O74">
         <v>404</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P74" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>62208</v>
       </c>
@@ -6640,7 +6787,7 @@
       <c r="J75" t="s">
         <v>20</v>
       </c>
-      <c r="K75" t="s">
+      <c r="K75" s="4" t="s">
         <v>216</v>
       </c>
       <c r="L75" t="s">
@@ -6655,8 +6802,14 @@
       <c r="O75">
         <v>404</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P75" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>61769</v>
       </c>
@@ -6687,7 +6840,7 @@
       <c r="J76" t="s">
         <v>220</v>
       </c>
-      <c r="K76" t="s">
+      <c r="K76" s="4" t="s">
         <v>219</v>
       </c>
       <c r="L76" t="s">
@@ -6702,8 +6855,11 @@
       <c r="O76">
         <v>404</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>58364</v>
       </c>
@@ -6734,7 +6890,7 @@
       <c r="J77" t="s">
         <v>20</v>
       </c>
-      <c r="K77" t="s">
+      <c r="K77" s="4" t="s">
         <v>222</v>
       </c>
       <c r="L77" t="s">
@@ -6749,8 +6905,14 @@
       <c r="O77">
         <v>404</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P77" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>57891</v>
       </c>
@@ -6781,7 +6943,7 @@
       <c r="J78" t="s">
         <v>20</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K78" s="4" t="s">
         <v>224</v>
       </c>
       <c r="L78" t="s">
@@ -6796,8 +6958,11 @@
       <c r="O78">
         <v>404</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>57782</v>
       </c>
@@ -6828,7 +6993,7 @@
       <c r="J79" t="s">
         <v>20</v>
       </c>
-      <c r="K79" t="s">
+      <c r="K79" s="4" t="s">
         <v>226</v>
       </c>
       <c r="L79" t="s">
@@ -6843,8 +7008,14 @@
       <c r="O79">
         <v>404</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P79" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>56563</v>
       </c>
@@ -6875,7 +7046,7 @@
       <c r="J80" t="s">
         <v>20</v>
       </c>
-      <c r="K80" t="s">
+      <c r="K80" s="4" t="s">
         <v>229</v>
       </c>
       <c r="L80" t="s">
@@ -6890,8 +7061,14 @@
       <c r="O80">
         <v>404</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P80" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>56112</v>
       </c>
@@ -6922,7 +7099,7 @@
       <c r="J81" t="s">
         <v>20</v>
       </c>
-      <c r="K81" t="s">
+      <c r="K81" s="4" t="s">
         <v>231</v>
       </c>
       <c r="L81" t="s">
@@ -6937,8 +7114,11 @@
       <c r="O81">
         <v>404</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>55090</v>
       </c>
@@ -6969,7 +7149,7 @@
       <c r="J82" t="s">
         <v>20</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K82" s="4" t="s">
         <v>235</v>
       </c>
       <c r="L82" t="s">
@@ -6984,8 +7164,14 @@
       <c r="O82">
         <v>404</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P82" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>54077</v>
       </c>
@@ -7016,7 +7202,7 @@
       <c r="J83" t="s">
         <v>20</v>
       </c>
-      <c r="K83" t="s">
+      <c r="K83" s="4" t="s">
         <v>237</v>
       </c>
       <c r="L83" t="s">
@@ -7031,8 +7217,11 @@
       <c r="O83">
         <v>404</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>54074</v>
       </c>
@@ -7063,7 +7252,7 @@
       <c r="J84" t="s">
         <v>20</v>
       </c>
-      <c r="K84" t="s">
+      <c r="K84" s="4" t="s">
         <v>241</v>
       </c>
       <c r="L84" t="s">
@@ -7078,8 +7267,14 @@
       <c r="O84">
         <v>404</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P84" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>53768</v>
       </c>
@@ -7110,7 +7305,7 @@
       <c r="J85" t="s">
         <v>20</v>
       </c>
-      <c r="K85" t="s">
+      <c r="K85" s="4" t="s">
         <v>243</v>
       </c>
       <c r="L85" t="s">
@@ -7125,8 +7320,11 @@
       <c r="O85">
         <v>404</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>53338</v>
       </c>
@@ -7157,7 +7355,7 @@
       <c r="J86" t="s">
         <v>20</v>
       </c>
-      <c r="K86" t="s">
+      <c r="K86" s="4" t="s">
         <v>247</v>
       </c>
       <c r="L86" t="s">
@@ -7172,8 +7370,14 @@
       <c r="O86">
         <v>404</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P86" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>52005</v>
       </c>
@@ -7204,7 +7408,7 @@
       <c r="J87" t="s">
         <v>20</v>
       </c>
-      <c r="K87" t="s">
+      <c r="K87" s="4" t="s">
         <v>249</v>
       </c>
       <c r="L87" t="s">
@@ -7219,8 +7423,14 @@
       <c r="O87">
         <v>404</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P87" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>51905</v>
       </c>
@@ -7251,7 +7461,7 @@
       <c r="J88" t="s">
         <v>20</v>
       </c>
-      <c r="K88" t="s">
+      <c r="K88" s="4" t="s">
         <v>252</v>
       </c>
       <c r="L88" t="s">
@@ -7266,8 +7476,14 @@
       <c r="O88">
         <v>404</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P88" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>51854</v>
       </c>
@@ -7298,7 +7514,7 @@
       <c r="J89" t="s">
         <v>20</v>
       </c>
-      <c r="K89" t="s">
+      <c r="K89" s="4" t="s">
         <v>255</v>
       </c>
       <c r="L89" t="s">
@@ -7313,8 +7529,14 @@
       <c r="O89">
         <v>404</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P89" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>51806</v>
       </c>
@@ -7345,7 +7567,7 @@
       <c r="J90" t="s">
         <v>20</v>
       </c>
-      <c r="K90" t="s">
+      <c r="K90" s="4" t="s">
         <v>257</v>
       </c>
       <c r="L90" t="s">
@@ -7360,8 +7582,14 @@
       <c r="O90">
         <v>404</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P90" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>50494</v>
       </c>
@@ -7392,7 +7620,7 @@
       <c r="J91" t="s">
         <v>20</v>
       </c>
-      <c r="K91" t="s">
+      <c r="K91" s="4" t="s">
         <v>259</v>
       </c>
       <c r="L91" t="s">
@@ -7407,8 +7635,11 @@
       <c r="O91">
         <v>404</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>50244</v>
       </c>
@@ -7439,7 +7670,7 @@
       <c r="J92" t="s">
         <v>20</v>
       </c>
-      <c r="K92" t="s">
+      <c r="K92" s="4" t="s">
         <v>262</v>
       </c>
       <c r="L92" t="s">
@@ -7454,8 +7685,14 @@
       <c r="O92">
         <v>404</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P92" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>50207</v>
       </c>
@@ -7486,7 +7723,7 @@
       <c r="J93" t="s">
         <v>20</v>
       </c>
-      <c r="K93" t="s">
+      <c r="K93" s="4" t="s">
         <v>265</v>
       </c>
       <c r="L93" t="s">
@@ -7501,8 +7738,14 @@
       <c r="O93">
         <v>404</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P93" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>49280</v>
       </c>
@@ -7533,7 +7776,7 @@
       <c r="J94" t="s">
         <v>20</v>
       </c>
-      <c r="K94" t="s">
+      <c r="K94" s="4" t="s">
         <v>268</v>
       </c>
       <c r="L94" t="s">
@@ -7548,8 +7791,11 @@
       <c r="O94">
         <v>404</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>48854</v>
       </c>
@@ -7580,7 +7826,7 @@
       <c r="J95" t="s">
         <v>20</v>
       </c>
-      <c r="K95" t="s">
+      <c r="K95" s="4" t="s">
         <v>271</v>
       </c>
       <c r="L95" t="s">
@@ -7595,8 +7841,14 @@
       <c r="O95">
         <v>404</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P95" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>46565</v>
       </c>
@@ -7627,7 +7879,7 @@
       <c r="J96" t="s">
         <v>20</v>
       </c>
-      <c r="K96" t="s">
+      <c r="K96" s="4" t="s">
         <v>274</v>
       </c>
       <c r="L96" t="s">
@@ -7642,8 +7894,14 @@
       <c r="O96">
         <v>404</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P96" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>46549</v>
       </c>
@@ -7674,7 +7932,7 @@
       <c r="J97" t="s">
         <v>20</v>
       </c>
-      <c r="K97" t="s">
+      <c r="K97" s="4" t="s">
         <v>276</v>
       </c>
       <c r="L97" t="s">
@@ -7689,8 +7947,14 @@
       <c r="O97">
         <v>404</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P97" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>46426</v>
       </c>
@@ -7721,7 +7985,7 @@
       <c r="J98" t="s">
         <v>279</v>
       </c>
-      <c r="K98" t="s">
+      <c r="K98" s="4" t="s">
         <v>278</v>
       </c>
       <c r="L98" t="s">
@@ -7736,8 +8000,11 @@
       <c r="O98">
         <v>404</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>46336</v>
       </c>
@@ -7768,7 +8035,7 @@
       <c r="J99" t="s">
         <v>20</v>
       </c>
-      <c r="K99" t="s">
+      <c r="K99" s="4" t="s">
         <v>281</v>
       </c>
       <c r="L99" t="s">
@@ -7783,8 +8050,14 @@
       <c r="O99">
         <v>404</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P99" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>46175</v>
       </c>
@@ -7815,7 +8088,7 @@
       <c r="J100" t="s">
         <v>285</v>
       </c>
-      <c r="K100" t="s">
+      <c r="K100" s="4" t="s">
         <v>283</v>
       </c>
       <c r="L100" t="s">
@@ -7830,8 +8103,14 @@
       <c r="O100">
         <v>404</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P100" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>46074</v>
       </c>
@@ -7862,7 +8141,7 @@
       <c r="J101" t="s">
         <v>20</v>
       </c>
-      <c r="K101" t="s">
+      <c r="K101" s="4" t="s">
         <v>287</v>
       </c>
       <c r="L101" t="s">
@@ -7877,8 +8156,14 @@
       <c r="O101">
         <v>404</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P101" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>46073</v>
       </c>
@@ -7909,7 +8194,7 @@
       <c r="J102" t="s">
         <v>20</v>
       </c>
-      <c r="K102" t="s">
+      <c r="K102" s="4" t="s">
         <v>289</v>
       </c>
       <c r="L102" t="s">
@@ -7924,8 +8209,14 @@
       <c r="O102">
         <v>404</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P102" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>45021</v>
       </c>
@@ -7956,7 +8247,7 @@
       <c r="J103" t="s">
         <v>20</v>
       </c>
-      <c r="K103" t="s">
+      <c r="K103" s="4" t="s">
         <v>291</v>
       </c>
       <c r="L103" t="s">
@@ -7971,8 +8262,14 @@
       <c r="O103">
         <v>404</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P103" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>34526</v>
       </c>
@@ -8003,7 +8300,7 @@
       <c r="J104" t="s">
         <v>20</v>
       </c>
-      <c r="K104" t="s">
+      <c r="K104" s="4" t="s">
         <v>293</v>
       </c>
       <c r="L104" t="s">
@@ -8018,8 +8315,14 @@
       <c r="O104">
         <v>404</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P104" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>17376</v>
       </c>
@@ -8050,7 +8353,7 @@
       <c r="J105" t="s">
         <v>20</v>
       </c>
-      <c r="K105" t="s">
+      <c r="K105" s="4" t="s">
         <v>295</v>
       </c>
       <c r="L105" t="s">
@@ -8065,8 +8368,11 @@
       <c r="O105">
         <v>404</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>12246</v>
       </c>
@@ -8097,7 +8403,7 @@
       <c r="J106" t="s">
         <v>20</v>
       </c>
-      <c r="K106" t="s">
+      <c r="K106" s="4" t="s">
         <v>298</v>
       </c>
       <c r="L106" t="s">
@@ -8112,8 +8418,14 @@
       <c r="O106">
         <v>404</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P106" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>9668</v>
       </c>
@@ -8144,7 +8456,7 @@
       <c r="J107" t="s">
         <v>20</v>
       </c>
-      <c r="K107" t="s">
+      <c r="K107" s="4" t="s">
         <v>300</v>
       </c>
       <c r="L107" t="s">
@@ -8159,8 +8471,14 @@
       <c r="O107">
         <v>404</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P107" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>113975</v>
       </c>
@@ -8191,7 +8509,7 @@
       <c r="J108" t="s">
         <v>20</v>
       </c>
-      <c r="K108" t="s">
+      <c r="K108" s="4" t="s">
         <v>302</v>
       </c>
       <c r="L108" t="s">
@@ -8206,8 +8524,11 @@
       <c r="O108">
         <v>404</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>113495</v>
       </c>
@@ -8238,7 +8559,7 @@
       <c r="J109" t="s">
         <v>20</v>
       </c>
-      <c r="K109" t="s">
+      <c r="K109" s="4" t="s">
         <v>306</v>
       </c>
       <c r="L109" t="s">
@@ -8253,8 +8574,11 @@
       <c r="O109">
         <v>404</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>113463</v>
       </c>
@@ -8285,7 +8609,7 @@
       <c r="J110" t="s">
         <v>20</v>
       </c>
-      <c r="K110" t="s">
+      <c r="K110" s="4" t="s">
         <v>310</v>
       </c>
       <c r="L110" t="s">
@@ -8300,8 +8624,11 @@
       <c r="O110">
         <v>404</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>113440</v>
       </c>
@@ -8332,7 +8659,7 @@
       <c r="J111" t="s">
         <v>20</v>
       </c>
-      <c r="K111" t="s">
+      <c r="K111" s="4" t="s">
         <v>314</v>
       </c>
       <c r="L111" t="s">
@@ -8347,8 +8674,11 @@
       <c r="O111">
         <v>404</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>112361</v>
       </c>
@@ -8379,7 +8709,7 @@
       <c r="J112" t="s">
         <v>20</v>
       </c>
-      <c r="K112" t="s">
+      <c r="K112" s="4" t="s">
         <v>318</v>
       </c>
       <c r="L112" t="s">
@@ -8394,8 +8724,11 @@
       <c r="O112">
         <v>404</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112331</v>
       </c>
@@ -8426,7 +8759,7 @@
       <c r="J113" t="s">
         <v>20</v>
       </c>
-      <c r="K113" t="s">
+      <c r="K113" s="4" t="s">
         <v>321</v>
       </c>
       <c r="L113" t="s">
@@ -8441,8 +8774,11 @@
       <c r="O113">
         <v>404</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>111883</v>
       </c>
@@ -8473,7 +8809,7 @@
       <c r="J114" t="s">
         <v>20</v>
       </c>
-      <c r="K114" t="s">
+      <c r="K114" s="4" t="s">
         <v>325</v>
       </c>
       <c r="L114" t="s">
@@ -8488,8 +8824,11 @@
       <c r="O114">
         <v>404</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>110170</v>
       </c>
@@ -8520,7 +8859,7 @@
       <c r="J115" t="s">
         <v>20</v>
       </c>
-      <c r="K115" t="s">
+      <c r="K115" s="4" t="s">
         <v>329</v>
       </c>
       <c r="L115" t="s">
@@ -8535,8 +8874,11 @@
       <c r="O115">
         <v>404</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>110170</v>
       </c>
@@ -8567,7 +8909,7 @@
       <c r="J116" t="s">
         <v>20</v>
       </c>
-      <c r="K116" t="s">
+      <c r="K116" s="4" t="s">
         <v>332</v>
       </c>
       <c r="L116" t="s">
@@ -8582,8 +8924,11 @@
       <c r="O116">
         <v>404</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>109944</v>
       </c>
@@ -8614,7 +8959,7 @@
       <c r="J117" t="s">
         <v>20</v>
       </c>
-      <c r="K117" t="s">
+      <c r="K117" s="4" t="s">
         <v>336</v>
       </c>
       <c r="L117" t="s">
@@ -8629,8 +8974,11 @@
       <c r="O117">
         <v>404</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>109816</v>
       </c>
@@ -8661,7 +9009,7 @@
       <c r="J118" t="s">
         <v>20</v>
       </c>
-      <c r="K118" t="s">
+      <c r="K118" s="4" t="s">
         <v>340</v>
       </c>
       <c r="L118" t="s">
@@ -8676,8 +9024,11 @@
       <c r="O118">
         <v>404</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>109468</v>
       </c>
@@ -8708,7 +9059,7 @@
       <c r="J119" t="s">
         <v>20</v>
       </c>
-      <c r="K119" t="s">
+      <c r="K119" s="4" t="s">
         <v>344</v>
       </c>
       <c r="L119" t="s">
@@ -8723,8 +9074,11 @@
       <c r="O119">
         <v>404</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>109424</v>
       </c>
@@ -8755,7 +9109,7 @@
       <c r="J120" t="s">
         <v>20</v>
       </c>
-      <c r="K120" t="s">
+      <c r="K120" s="4" t="s">
         <v>348</v>
       </c>
       <c r="L120" t="s">
@@ -8770,8 +9124,11 @@
       <c r="O120">
         <v>404</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>108253</v>
       </c>
@@ -8802,7 +9159,7 @@
       <c r="J121" t="s">
         <v>20</v>
       </c>
-      <c r="K121" t="s">
+      <c r="K121" s="4" t="s">
         <v>352</v>
       </c>
       <c r="L121" t="s">
@@ -8817,8 +9174,17 @@
       <c r="O121">
         <v>404</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P121" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>672</v>
+      </c>
+      <c r="R121" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>108119</v>
       </c>
@@ -8849,7 +9215,7 @@
       <c r="J122" t="s">
         <v>20</v>
       </c>
-      <c r="K122" t="s">
+      <c r="K122" s="4" t="s">
         <v>354</v>
       </c>
       <c r="L122" t="s">
@@ -8864,8 +9230,14 @@
       <c r="O122">
         <v>404</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P122" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>108005</v>
       </c>
@@ -8896,7 +9268,7 @@
       <c r="J123" t="s">
         <v>20</v>
       </c>
-      <c r="K123" t="s">
+      <c r="K123" s="4" t="s">
         <v>358</v>
       </c>
       <c r="L123" t="s">
@@ -8911,8 +9283,17 @@
       <c r="O123">
         <v>404</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P123" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>672</v>
+      </c>
+      <c r="R123" s="4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>107876</v>
       </c>
@@ -8943,7 +9324,7 @@
       <c r="J124" t="s">
         <v>20</v>
       </c>
-      <c r="K124" t="s">
+      <c r="K124" s="4" t="s">
         <v>362</v>
       </c>
       <c r="L124" t="s">
@@ -8958,8 +9339,11 @@
       <c r="O124">
         <v>404</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>107587</v>
       </c>
@@ -8990,7 +9374,7 @@
       <c r="J125" t="s">
         <v>20</v>
       </c>
-      <c r="K125" t="s">
+      <c r="K125" s="4" t="s">
         <v>366</v>
       </c>
       <c r="L125" t="s">
@@ -9005,8 +9389,11 @@
       <c r="O125">
         <v>404</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>107463</v>
       </c>
@@ -9037,7 +9424,7 @@
       <c r="J126" t="s">
         <v>20</v>
       </c>
-      <c r="K126" t="s">
+      <c r="K126" s="4" t="s">
         <v>370</v>
       </c>
       <c r="L126" t="s">
@@ -9052,8 +9439,11 @@
       <c r="O126">
         <v>404</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>105752</v>
       </c>
@@ -9084,7 +9474,7 @@
       <c r="J127" t="s">
         <v>20</v>
       </c>
-      <c r="K127" t="s">
+      <c r="K127" s="4" t="s">
         <v>374</v>
       </c>
       <c r="L127" t="s">
@@ -9099,8 +9489,11 @@
       <c r="O127">
         <v>404</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>105752</v>
       </c>
@@ -9131,7 +9524,7 @@
       <c r="J128" t="s">
         <v>20</v>
       </c>
-      <c r="K128" t="s">
+      <c r="K128" s="4" t="s">
         <v>375</v>
       </c>
       <c r="L128" t="s">
@@ -9146,8 +9539,11 @@
       <c r="O128">
         <v>404</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>105256</v>
       </c>
@@ -9178,7 +9574,7 @@
       <c r="J129" t="s">
         <v>20</v>
       </c>
-      <c r="K129" t="s">
+      <c r="K129" s="4" t="s">
         <v>379</v>
       </c>
       <c r="L129" t="s">
@@ -9193,8 +9589,17 @@
       <c r="O129">
         <v>404</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P129" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>672</v>
+      </c>
+      <c r="R129" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>105116</v>
       </c>
@@ -9225,7 +9630,7 @@
       <c r="J130" t="s">
         <v>20</v>
       </c>
-      <c r="K130" t="s">
+      <c r="K130" s="4" t="s">
         <v>383</v>
       </c>
       <c r="L130" t="s">
@@ -9240,8 +9645,11 @@
       <c r="O130">
         <v>404</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>104183</v>
       </c>
@@ -9272,7 +9680,7 @@
       <c r="J131" t="s">
         <v>20</v>
       </c>
-      <c r="K131" t="s">
+      <c r="K131" s="4" t="s">
         <v>387</v>
       </c>
       <c r="L131" t="s">
@@ -9287,8 +9695,11 @@
       <c r="O131">
         <v>404</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>101062</v>
       </c>
@@ -9319,7 +9730,7 @@
       <c r="J132" t="s">
         <v>20</v>
       </c>
-      <c r="K132" t="s">
+      <c r="K132" s="4" t="s">
         <v>391</v>
       </c>
       <c r="L132" t="s">
@@ -9334,8 +9745,11 @@
       <c r="O132">
         <v>404</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>92247</v>
       </c>
@@ -9366,7 +9780,7 @@
       <c r="J133" t="s">
         <v>20</v>
       </c>
-      <c r="K133" t="s">
+      <c r="K133" s="4" t="s">
         <v>393</v>
       </c>
       <c r="L133" t="s">
@@ -9381,8 +9795,11 @@
       <c r="O133">
         <v>404</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>92026</v>
       </c>
@@ -9413,7 +9830,7 @@
       <c r="J134" t="s">
         <v>20</v>
       </c>
-      <c r="K134" t="s">
+      <c r="K134" s="4" t="s">
         <v>397</v>
       </c>
       <c r="L134" t="s">
@@ -9428,8 +9845,11 @@
       <c r="O134">
         <v>404</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>72209</v>
       </c>
@@ -9460,7 +9880,7 @@
       <c r="J135" t="s">
         <v>20</v>
       </c>
-      <c r="K135" t="s">
+      <c r="K135" s="4" t="s">
         <v>401</v>
       </c>
       <c r="L135" t="s">
@@ -9475,8 +9895,11 @@
       <c r="O135">
         <v>404</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>70137</v>
       </c>
@@ -9507,7 +9930,7 @@
       <c r="J136" t="s">
         <v>20</v>
       </c>
-      <c r="K136" t="s">
+      <c r="K136" s="4" t="s">
         <v>405</v>
       </c>
       <c r="L136" t="s">
@@ -9522,8 +9945,11 @@
       <c r="O136">
         <v>404</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>61552</v>
       </c>
@@ -9554,7 +9980,7 @@
       <c r="J137" t="s">
         <v>20</v>
       </c>
-      <c r="K137" t="s">
+      <c r="K137" s="4" t="s">
         <v>409</v>
       </c>
       <c r="L137" t="s">
@@ -9569,8 +9995,11 @@
       <c r="O137">
         <v>404</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>116260</v>
       </c>
@@ -9601,7 +10030,7 @@
       <c r="J138" t="s">
         <v>93</v>
       </c>
-      <c r="K138" t="s">
+      <c r="K138" s="4" t="s">
         <v>413</v>
       </c>
       <c r="L138" t="s">
@@ -9616,8 +10045,14 @@
       <c r="O138">
         <v>404</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P138" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>111605</v>
       </c>
@@ -9648,7 +10083,7 @@
       <c r="J139" t="s">
         <v>417</v>
       </c>
-      <c r="K139" t="s">
+      <c r="K139" s="4" t="s">
         <v>418</v>
       </c>
       <c r="L139" t="s">
@@ -9663,8 +10098,14 @@
       <c r="O139">
         <v>404</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P139" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>111177</v>
       </c>
@@ -9695,7 +10136,7 @@
       <c r="J140" t="s">
         <v>421</v>
       </c>
-      <c r="K140" t="s">
+      <c r="K140" s="4" t="s">
         <v>422</v>
       </c>
       <c r="L140" t="s">
@@ -9710,8 +10151,14 @@
       <c r="O140">
         <v>404</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P140" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>109556</v>
       </c>
@@ -9742,7 +10189,7 @@
       <c r="J141" t="s">
         <v>425</v>
       </c>
-      <c r="K141" t="s">
+      <c r="K141" s="4" t="s">
         <v>426</v>
       </c>
       <c r="L141" t="s">
@@ -9757,8 +10204,14 @@
       <c r="O141">
         <v>404</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P141" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>108168</v>
       </c>
@@ -9789,7 +10242,7 @@
       <c r="J142" t="s">
         <v>417</v>
       </c>
-      <c r="K142" t="s">
+      <c r="K142" s="4" t="s">
         <v>429</v>
       </c>
       <c r="L142" t="s">
@@ -9804,8 +10257,14 @@
       <c r="O142">
         <v>404</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P142" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>106221</v>
       </c>
@@ -9836,7 +10295,7 @@
       <c r="J143" t="s">
         <v>432</v>
       </c>
-      <c r="K143" t="s">
+      <c r="K143" s="4" t="s">
         <v>433</v>
       </c>
       <c r="L143" t="s">
@@ -9851,8 +10310,14 @@
       <c r="O143">
         <v>404</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P143" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>103512</v>
       </c>
@@ -9883,7 +10348,7 @@
       <c r="J144" t="s">
         <v>436</v>
       </c>
-      <c r="K144" t="s">
+      <c r="K144" s="4" t="s">
         <v>437</v>
       </c>
       <c r="L144" t="s">
@@ -9898,8 +10363,11 @@
       <c r="O144">
         <v>404</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>102428</v>
       </c>
@@ -9930,7 +10398,7 @@
       <c r="J145" t="s">
         <v>439</v>
       </c>
-      <c r="K145" t="s">
+      <c r="K145" s="4" t="s">
         <v>440</v>
       </c>
       <c r="L145" t="s">
@@ -9945,8 +10413,14 @@
       <c r="O145">
         <v>404</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P145" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>102411</v>
       </c>
@@ -9977,7 +10451,7 @@
       <c r="J146" t="s">
         <v>443</v>
       </c>
-      <c r="K146" t="s">
+      <c r="K146" s="4" t="s">
         <v>444</v>
       </c>
       <c r="L146" t="s">
@@ -9992,8 +10466,14 @@
       <c r="O146">
         <v>404</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P146" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>100825</v>
       </c>
@@ -10024,7 +10504,7 @@
       <c r="J147" t="s">
         <v>417</v>
       </c>
-      <c r="K147" t="s">
+      <c r="K147" s="4" t="s">
         <v>447</v>
       </c>
       <c r="L147" t="s">
@@ -10039,8 +10519,14 @@
       <c r="O147">
         <v>404</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P147" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>67048</v>
       </c>
@@ -10071,7 +10557,7 @@
       <c r="J148" t="s">
         <v>450</v>
       </c>
-      <c r="K148" t="s">
+      <c r="K148" s="4" t="s">
         <v>451</v>
       </c>
       <c r="L148" t="s">
@@ -10086,8 +10572,14 @@
       <c r="O148">
         <v>404</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P148" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>106838</v>
       </c>
@@ -10118,7 +10610,7 @@
       <c r="J149" t="s">
         <v>454</v>
       </c>
-      <c r="K149" t="s">
+      <c r="K149" s="4" t="s">
         <v>455</v>
       </c>
       <c r="L149" t="s">
@@ -10133,8 +10625,14 @@
       <c r="O149">
         <v>404</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P149" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>106838</v>
       </c>
@@ -10165,7 +10663,7 @@
       <c r="J150" t="s">
         <v>454</v>
       </c>
-      <c r="K150" t="s">
+      <c r="K150" s="4" t="s">
         <v>458</v>
       </c>
       <c r="L150" t="s">
@@ -10180,8 +10678,14 @@
       <c r="O150">
         <v>404</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P150" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>106838</v>
       </c>
@@ -10212,7 +10716,7 @@
       <c r="J151" t="s">
         <v>454</v>
       </c>
-      <c r="K151" t="s">
+      <c r="K151" s="4" t="s">
         <v>461</v>
       </c>
       <c r="L151" t="s">
@@ -10227,8 +10731,14 @@
       <c r="O151">
         <v>404</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P151" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>93010</v>
       </c>
@@ -10259,7 +10769,7 @@
       <c r="J152" t="s">
         <v>465</v>
       </c>
-      <c r="K152" t="s">
+      <c r="K152" s="4" t="s">
         <v>466</v>
       </c>
       <c r="L152" t="s">
@@ -10274,8 +10784,14 @@
       <c r="O152">
         <v>404</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P152" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>83929</v>
       </c>
@@ -10306,7 +10822,7 @@
       <c r="J153" t="s">
         <v>432</v>
       </c>
-      <c r="K153" t="s">
+      <c r="K153" s="4" t="s">
         <v>470</v>
       </c>
       <c r="L153" t="s">
@@ -10321,8 +10837,17 @@
       <c r="O153">
         <v>404</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P153" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>672</v>
+      </c>
+      <c r="R153" s="4" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>109524</v>
       </c>
@@ -10353,7 +10878,7 @@
       <c r="J154" t="s">
         <v>20</v>
       </c>
-      <c r="K154" t="s">
+      <c r="K154" s="4" t="s">
         <v>472</v>
       </c>
       <c r="L154" t="s">
@@ -10368,8 +10893,17 @@
       <c r="O154" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P154" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q154" t="s">
+        <v>672</v>
+      </c>
+      <c r="R154" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>105482</v>
       </c>
@@ -10400,7 +10934,7 @@
       <c r="J155" t="s">
         <v>20</v>
       </c>
-      <c r="K155" t="s">
+      <c r="K155" s="4" t="s">
         <v>474</v>
       </c>
       <c r="L155" t="s">
@@ -10415,8 +10949,17 @@
       <c r="O155" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P155" t="s">
+        <v>678</v>
+      </c>
+      <c r="Q155" t="s">
+        <v>672</v>
+      </c>
+      <c r="R155" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>99276</v>
       </c>
@@ -10447,7 +10990,7 @@
       <c r="J156" t="s">
         <v>450</v>
       </c>
-      <c r="K156" t="s">
+      <c r="K156" s="4" t="s">
         <v>476</v>
       </c>
       <c r="L156" t="s">
@@ -10462,8 +11005,15 @@
       <c r="O156" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P156" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>699</v>
+      </c>
+      <c r="R156" s="4"/>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>111276</v>
       </c>
@@ -10494,7 +11044,7 @@
       <c r="J157" t="s">
         <v>20</v>
       </c>
-      <c r="K157" t="s">
+      <c r="K157" s="4" t="s">
         <v>479</v>
       </c>
       <c r="L157" t="s">
@@ -10509,8 +11059,11 @@
       <c r="O157" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>111607</v>
       </c>
@@ -10541,7 +11094,7 @@
       <c r="J158" t="s">
         <v>20</v>
       </c>
-      <c r="K158" t="s">
+      <c r="K158" s="4" t="s">
         <v>482</v>
       </c>
       <c r="L158" t="s">
@@ -10556,8 +11109,11 @@
       <c r="O158" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>110848</v>
       </c>
@@ -10588,7 +11144,7 @@
       <c r="J159" t="s">
         <v>20</v>
       </c>
-      <c r="K159" t="s">
+      <c r="K159" s="4" t="s">
         <v>486</v>
       </c>
       <c r="L159" t="s">
@@ -10603,8 +11159,11 @@
       <c r="O159" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>112933</v>
       </c>
@@ -10635,7 +11194,7 @@
       <c r="J160" t="s">
         <v>20</v>
       </c>
-      <c r="K160" t="s">
+      <c r="K160" s="4" t="s">
         <v>489</v>
       </c>
       <c r="L160" t="s">
@@ -10650,8 +11209,11 @@
       <c r="O160" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>115997</v>
       </c>
@@ -10682,7 +11244,7 @@
       <c r="J161" t="s">
         <v>495</v>
       </c>
-      <c r="K161" t="s">
+      <c r="K161" s="4" t="s">
         <v>493</v>
       </c>
       <c r="L161" t="s">
@@ -10697,8 +11259,11 @@
       <c r="O161" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>114815</v>
       </c>
@@ -10729,7 +11294,7 @@
       <c r="J162" t="s">
         <v>20</v>
       </c>
-      <c r="K162" t="s">
+      <c r="K162" s="4" t="s">
         <v>498</v>
       </c>
       <c r="L162" t="s">
@@ -10744,8 +11309,11 @@
       <c r="O162" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P162" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>115863</v>
       </c>
@@ -10776,7 +11344,7 @@
       <c r="J163" t="s">
         <v>20</v>
       </c>
-      <c r="K163" t="s">
+      <c r="K163" s="4" t="s">
         <v>501</v>
       </c>
       <c r="L163" t="s">
@@ -10791,8 +11359,11 @@
       <c r="O163" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>115017</v>
       </c>
@@ -10823,7 +11394,7 @@
       <c r="J164" t="s">
         <v>20</v>
       </c>
-      <c r="K164" t="s">
+      <c r="K164" s="4" t="s">
         <v>504</v>
       </c>
       <c r="L164" t="s">
@@ -10838,8 +11409,11 @@
       <c r="O164" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P164" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>86225</v>
       </c>
@@ -10870,7 +11444,7 @@
       <c r="J165" t="s">
         <v>20</v>
       </c>
-      <c r="K165" t="s">
+      <c r="K165" s="4" t="s">
         <v>506</v>
       </c>
       <c r="L165" t="s">
@@ -10885,8 +11459,11 @@
       <c r="O165" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>83453</v>
       </c>
@@ -10917,7 +11494,7 @@
       <c r="J166" t="s">
         <v>20</v>
       </c>
-      <c r="K166" t="s">
+      <c r="K166" s="4" t="s">
         <v>509</v>
       </c>
       <c r="L166" t="s">
@@ -10932,15 +11509,18 @@
       <c r="O166" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P166" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>59910</v>
       </c>
       <c r="B167" t="s">
         <v>510</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="4" t="s">
         <v>511</v>
       </c>
       <c r="D167" t="s">
@@ -10964,7 +11544,7 @@
       <c r="J167" t="s">
         <v>20</v>
       </c>
-      <c r="K167" t="s">
+      <c r="K167" s="4" t="s">
         <v>511</v>
       </c>
       <c r="L167" t="s">
@@ -10979,8 +11559,11 @@
       <c r="O167" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>114950</v>
       </c>
@@ -11011,7 +11594,7 @@
       <c r="J168" t="s">
         <v>20</v>
       </c>
-      <c r="K168" t="s">
+      <c r="K168" s="4" t="s">
         <v>514</v>
       </c>
       <c r="L168" t="s">
@@ -11026,8 +11609,11 @@
       <c r="O168" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P168" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>114883</v>
       </c>
@@ -11058,7 +11644,7 @@
       <c r="J169" t="s">
         <v>20</v>
       </c>
-      <c r="K169" t="s">
+      <c r="K169" s="4" t="s">
         <v>517</v>
       </c>
       <c r="L169" t="s">
@@ -11073,8 +11659,11 @@
       <c r="O169" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P169" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>114745</v>
       </c>
@@ -11105,7 +11694,7 @@
       <c r="J170" t="s">
         <v>20</v>
       </c>
-      <c r="K170" t="s">
+      <c r="K170" s="4" t="s">
         <v>519</v>
       </c>
       <c r="L170" t="s">
@@ -11120,8 +11709,11 @@
       <c r="O170" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P170" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>114743</v>
       </c>
@@ -11152,7 +11744,7 @@
       <c r="J171" t="s">
         <v>20</v>
       </c>
-      <c r="K171" t="s">
+      <c r="K171" s="4" t="s">
         <v>521</v>
       </c>
       <c r="L171" t="s">
@@ -11167,8 +11759,11 @@
       <c r="O171" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P171" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>115024</v>
       </c>
@@ -11199,7 +11794,7 @@
       <c r="J172" t="s">
         <v>526</v>
       </c>
-      <c r="K172" t="s">
+      <c r="K172" s="4" t="s">
         <v>523</v>
       </c>
       <c r="L172" t="s">
@@ -11214,8 +11809,11 @@
       <c r="O172" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P172" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>115024</v>
       </c>
@@ -11246,7 +11844,7 @@
       <c r="J173" t="s">
         <v>526</v>
       </c>
-      <c r="K173" t="s">
+      <c r="K173" s="4" t="s">
         <v>528</v>
       </c>
       <c r="L173" t="s">
@@ -11261,8 +11859,11 @@
       <c r="O173" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P173" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>115024</v>
       </c>
@@ -11293,7 +11894,7 @@
       <c r="J174" t="s">
         <v>526</v>
       </c>
-      <c r="K174" t="s">
+      <c r="K174" s="4" t="s">
         <v>530</v>
       </c>
       <c r="L174" t="s">
@@ -11308,8 +11909,11 @@
       <c r="O174" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P174" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>114752</v>
       </c>
@@ -11340,7 +11944,7 @@
       <c r="J175" t="s">
         <v>20</v>
       </c>
-      <c r="K175" t="s">
+      <c r="K175" s="4" t="s">
         <v>533</v>
       </c>
       <c r="L175" t="s">
@@ -11355,8 +11959,11 @@
       <c r="O175" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>114745</v>
       </c>
@@ -11387,7 +11994,7 @@
       <c r="J176" t="s">
         <v>20</v>
       </c>
-      <c r="K176" t="s">
+      <c r="K176" s="4" t="s">
         <v>535</v>
       </c>
       <c r="L176" t="s">
@@ -11402,8 +12009,11 @@
       <c r="O176" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P176" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>114729</v>
       </c>
@@ -11434,7 +12044,7 @@
       <c r="J177" t="s">
         <v>20</v>
       </c>
-      <c r="K177" t="s">
+      <c r="K177" s="4" t="s">
         <v>537</v>
       </c>
       <c r="L177" t="s">
@@ -11449,8 +12059,14 @@
       <c r="O177" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P177" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q177" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>85039</v>
       </c>
@@ -11481,7 +12097,7 @@
       <c r="J178" t="s">
         <v>20</v>
       </c>
-      <c r="K178" t="s">
+      <c r="K178" s="4" t="s">
         <v>541</v>
       </c>
       <c r="L178" t="s">
@@ -11496,8 +12112,14 @@
       <c r="O178" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P178" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q178" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>83811</v>
       </c>
@@ -11528,7 +12150,7 @@
       <c r="J179" t="s">
         <v>20</v>
       </c>
-      <c r="K179" t="s">
+      <c r="K179" s="4" t="s">
         <v>544</v>
       </c>
       <c r="L179" t="s">
@@ -11543,8 +12165,14 @@
       <c r="O179" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P179" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q179" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>82180</v>
       </c>
@@ -11575,7 +12203,7 @@
       <c r="J180" t="s">
         <v>20</v>
       </c>
-      <c r="K180" t="s">
+      <c r="K180" s="4" t="s">
         <v>547</v>
       </c>
       <c r="L180" t="s">
@@ -11590,8 +12218,14 @@
       <c r="O180" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P180" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q180" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>72399</v>
       </c>
@@ -11622,7 +12256,7 @@
       <c r="J181" t="s">
         <v>20</v>
       </c>
-      <c r="K181" t="s">
+      <c r="K181" s="4" t="s">
         <v>550</v>
       </c>
       <c r="L181" t="s">
@@ -11637,8 +12271,14 @@
       <c r="O181" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P181" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q181" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>60531</v>
       </c>
@@ -11669,7 +12309,7 @@
       <c r="J182" t="s">
         <v>20</v>
       </c>
-      <c r="K182" t="s">
+      <c r="K182" s="4" t="s">
         <v>553</v>
       </c>
       <c r="L182" t="s">
@@ -11684,8 +12324,11 @@
       <c r="O182" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P182" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>60404</v>
       </c>
@@ -11716,7 +12359,7 @@
       <c r="J183" t="s">
         <v>20</v>
       </c>
-      <c r="K183" t="s">
+      <c r="K183" s="4" t="s">
         <v>555</v>
       </c>
       <c r="L183" t="s">
@@ -11731,8 +12374,11 @@
       <c r="O183" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P183" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>59501</v>
       </c>
@@ -11763,7 +12409,7 @@
       <c r="J184" t="s">
         <v>20</v>
       </c>
-      <c r="K184" t="s">
+      <c r="K184" s="4" t="s">
         <v>557</v>
       </c>
       <c r="L184" t="s">
@@ -11778,8 +12424,11 @@
       <c r="O184" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P184" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>58276</v>
       </c>
@@ -11810,7 +12459,7 @@
       <c r="J185" t="s">
         <v>20</v>
       </c>
-      <c r="K185" t="s">
+      <c r="K185" s="4" t="s">
         <v>559</v>
       </c>
       <c r="L185" t="s">
@@ -11825,8 +12474,11 @@
       <c r="O185" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P185" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>115502</v>
       </c>
@@ -11857,7 +12509,7 @@
       <c r="J186" t="s">
         <v>20</v>
       </c>
-      <c r="K186" t="s">
+      <c r="K186" s="4" t="s">
         <v>560</v>
       </c>
       <c r="L186" t="s">
@@ -11872,8 +12524,11 @@
       <c r="O186" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P186" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>114740</v>
       </c>
@@ -11904,7 +12559,7 @@
       <c r="J187" t="s">
         <v>20</v>
       </c>
-      <c r="K187" t="s">
+      <c r="K187" s="4" t="s">
         <v>564</v>
       </c>
       <c r="L187" t="s">
@@ -11919,8 +12574,14 @@
       <c r="O187" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P187" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q187" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>106942</v>
       </c>
@@ -11951,7 +12612,7 @@
       <c r="J188" t="s">
         <v>20</v>
       </c>
-      <c r="K188" t="s">
+      <c r="K188" s="4" t="s">
         <v>567</v>
       </c>
       <c r="L188" t="s">
@@ -11966,8 +12627,14 @@
       <c r="O188" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P188" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q188" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>117947</v>
       </c>
@@ -11998,7 +12665,7 @@
       <c r="J189" t="s">
         <v>20</v>
       </c>
-      <c r="K189" t="s">
+      <c r="K189" s="4" t="s">
         <v>571</v>
       </c>
       <c r="L189" t="s">
@@ -12013,8 +12680,11 @@
       <c r="O189" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P189" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>115318</v>
       </c>
@@ -12045,7 +12715,7 @@
       <c r="J190" t="s">
         <v>578</v>
       </c>
-      <c r="K190" t="s">
+      <c r="K190" s="4" t="s">
         <v>575</v>
       </c>
       <c r="L190" t="s">
@@ -12060,8 +12730,14 @@
       <c r="O190" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P190" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q190" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>114601</v>
       </c>
@@ -12092,7 +12768,7 @@
       <c r="J191" t="s">
         <v>578</v>
       </c>
-      <c r="K191" t="s">
+      <c r="K191" s="4" t="s">
         <v>580</v>
       </c>
       <c r="L191" t="s">
@@ -12107,8 +12783,14 @@
       <c r="O191" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P191" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q191" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>99896</v>
       </c>
@@ -12139,7 +12821,7 @@
       <c r="J192" t="s">
         <v>20</v>
       </c>
-      <c r="K192" t="s">
+      <c r="K192" s="4" t="s">
         <v>583</v>
       </c>
       <c r="L192" t="s">
@@ -12154,8 +12836,11 @@
       <c r="O192" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P192" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>72621</v>
       </c>
@@ -12186,7 +12871,7 @@
       <c r="J193" t="s">
         <v>587</v>
       </c>
-      <c r="K193" t="s">
+      <c r="K193" s="4" t="s">
         <v>585</v>
       </c>
       <c r="L193" t="s">
@@ -12201,8 +12886,11 @@
       <c r="O193" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P193" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>68959</v>
       </c>
@@ -12233,7 +12921,7 @@
       <c r="J194" t="s">
         <v>20</v>
       </c>
-      <c r="K194" t="s">
+      <c r="K194" s="4" t="s">
         <v>589</v>
       </c>
       <c r="L194" t="s">
@@ -12248,8 +12936,11 @@
       <c r="O194" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P194" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>57144</v>
       </c>
@@ -12280,7 +12971,7 @@
       <c r="J195" t="s">
         <v>20</v>
       </c>
-      <c r="K195" t="s">
+      <c r="K195" s="4" t="s">
         <v>591</v>
       </c>
       <c r="L195" t="s">
@@ -12295,8 +12986,11 @@
       <c r="O195" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P195" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>50354</v>
       </c>
@@ -12327,7 +13021,7 @@
       <c r="J196" t="s">
         <v>20</v>
       </c>
-      <c r="K196" t="s">
+      <c r="K196" s="4" t="s">
         <v>593</v>
       </c>
       <c r="L196" t="s">
@@ -12342,8 +13036,11 @@
       <c r="O196" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P196" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>46094</v>
       </c>
@@ -12374,7 +13071,7 @@
       <c r="J197" t="s">
         <v>20</v>
       </c>
-      <c r="K197" t="s">
+      <c r="K197" s="4" t="s">
         <v>596</v>
       </c>
       <c r="L197" t="s">
@@ -12389,8 +13086,11 @@
       <c r="O197" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P197" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>43217</v>
       </c>
@@ -12421,7 +13121,7 @@
       <c r="J198" t="s">
         <v>20</v>
       </c>
-      <c r="K198" t="s">
+      <c r="K198" s="4" t="s">
         <v>599</v>
       </c>
       <c r="L198" t="s">
@@ -12436,8 +13136,11 @@
       <c r="O198" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P198" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>43217</v>
       </c>
@@ -12468,7 +13171,7 @@
       <c r="J199" t="s">
         <v>20</v>
       </c>
-      <c r="K199" t="s">
+      <c r="K199" s="4" t="s">
         <v>600</v>
       </c>
       <c r="L199" t="s">
@@ -12483,8 +13186,11 @@
       <c r="O199" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P199" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>43217</v>
       </c>
@@ -12515,7 +13221,7 @@
       <c r="J200" t="s">
         <v>20</v>
       </c>
-      <c r="K200" t="s">
+      <c r="K200" s="4" t="s">
         <v>601</v>
       </c>
       <c r="L200" t="s">
@@ -12530,8 +13236,11 @@
       <c r="O200" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P200" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>42875</v>
       </c>
@@ -12562,7 +13271,7 @@
       <c r="J201" t="s">
         <v>20</v>
       </c>
-      <c r="K201" t="s">
+      <c r="K201" s="4" t="s">
         <v>603</v>
       </c>
       <c r="L201" t="s">
@@ -12577,8 +13286,11 @@
       <c r="O201" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P201" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>29134</v>
       </c>
@@ -12609,7 +13321,7 @@
       <c r="J202" t="s">
         <v>20</v>
       </c>
-      <c r="K202" t="s">
+      <c r="K202" s="4" t="s">
         <v>606</v>
       </c>
       <c r="L202" t="s">
@@ -12624,8 +13336,11 @@
       <c r="O202" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P202" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>114752</v>
       </c>
@@ -12656,7 +13371,7 @@
       <c r="J203" t="s">
         <v>20</v>
       </c>
-      <c r="K203" t="s">
+      <c r="K203" s="4" t="s">
         <v>607</v>
       </c>
       <c r="L203" t="s">
@@ -12671,8 +13386,11 @@
       <c r="O203" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P203" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>113921</v>
       </c>
@@ -12703,7 +13421,7 @@
       <c r="J204" t="s">
         <v>20</v>
       </c>
-      <c r="K204" t="s">
+      <c r="K204" s="4" t="s">
         <v>609</v>
       </c>
       <c r="L204" t="s">
@@ -12718,8 +13436,11 @@
       <c r="O204" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P204" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>102324</v>
       </c>
@@ -12750,7 +13471,7 @@
       <c r="J205" t="s">
         <v>20</v>
       </c>
-      <c r="K205" t="s">
+      <c r="K205" s="4" t="s">
         <v>611</v>
       </c>
       <c r="L205" t="s">
@@ -12765,8 +13486,11 @@
       <c r="O205" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>108622</v>
       </c>
@@ -12797,7 +13521,7 @@
       <c r="J206" t="s">
         <v>20</v>
       </c>
-      <c r="K206" t="s">
+      <c r="K206" s="4" t="s">
         <v>616</v>
       </c>
       <c r="L206" t="s">
@@ -12812,8 +13536,11 @@
       <c r="O206" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P206" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>108622</v>
       </c>
@@ -12844,7 +13571,7 @@
       <c r="J207" t="s">
         <v>20</v>
       </c>
-      <c r="K207" t="s">
+      <c r="K207" s="4" t="s">
         <v>618</v>
       </c>
       <c r="L207" t="s">
@@ -12859,8 +13586,11 @@
       <c r="O207" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P207" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>116260</v>
       </c>
@@ -12891,7 +13621,7 @@
       <c r="J208" t="s">
         <v>20</v>
       </c>
-      <c r="K208" t="s">
+      <c r="K208" s="4" t="s">
         <v>619</v>
       </c>
       <c r="L208" t="s">
@@ -12906,8 +13636,11 @@
       <c r="O208" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P208" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>101743</v>
       </c>
@@ -12938,7 +13671,7 @@
       <c r="J209" t="s">
         <v>20</v>
       </c>
-      <c r="K209" t="s">
+      <c r="K209" s="4" t="s">
         <v>623</v>
       </c>
       <c r="L209" t="s">
@@ -12953,8 +13686,11 @@
       <c r="O209" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P209" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>110009</v>
       </c>
@@ -12985,7 +13721,7 @@
       <c r="J210" t="s">
         <v>20</v>
       </c>
-      <c r="K210" t="s">
+      <c r="K210" s="4" t="s">
         <v>626</v>
       </c>
       <c r="L210" t="s">
@@ -13000,8 +13736,11 @@
       <c r="O210" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P210" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>110009</v>
       </c>
@@ -13032,7 +13771,7 @@
       <c r="J211" t="s">
         <v>20</v>
       </c>
-      <c r="K211" t="s">
+      <c r="K211" s="4" t="s">
         <v>628</v>
       </c>
       <c r="L211" t="s">
@@ -13047,8 +13786,11 @@
       <c r="O211" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>110009</v>
       </c>
@@ -13079,7 +13821,7 @@
       <c r="J212" t="s">
         <v>20</v>
       </c>
-      <c r="K212" t="s">
+      <c r="K212" s="4" t="s">
         <v>629</v>
       </c>
       <c r="L212" t="s">
@@ -13094,15 +13836,21 @@
       <c r="O212" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P212" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q212" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>106266</v>
       </c>
       <c r="B213" t="s">
         <v>631</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C213" s="4" t="s">
         <v>632</v>
       </c>
       <c r="D213" t="s">
@@ -13126,7 +13874,7 @@
       <c r="J213" t="s">
         <v>20</v>
       </c>
-      <c r="K213" t="s">
+      <c r="K213" s="4" t="s">
         <v>632</v>
       </c>
       <c r="L213" t="s">
@@ -13141,8 +13889,14 @@
       <c r="O213" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P213" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q213" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>104501</v>
       </c>
@@ -13173,7 +13927,7 @@
       <c r="J214" t="s">
         <v>20</v>
       </c>
-      <c r="K214" t="s">
+      <c r="K214" s="4" t="s">
         <v>636</v>
       </c>
       <c r="L214" t="s">
@@ -13188,8 +13942,11 @@
       <c r="O214" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P214" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>97594</v>
       </c>
@@ -13220,7 +13977,7 @@
       <c r="J215" t="s">
         <v>20</v>
       </c>
-      <c r="K215" t="s">
+      <c r="K215" s="4" t="s">
         <v>638</v>
       </c>
       <c r="L215" t="s">
@@ -13235,15 +13992,18 @@
       <c r="O215" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P215" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>90629</v>
       </c>
       <c r="B216" t="s">
         <v>639</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="4" t="s">
         <v>640</v>
       </c>
       <c r="D216" t="s">
@@ -13267,7 +14027,7 @@
       <c r="J216" t="s">
         <v>20</v>
       </c>
-      <c r="K216" t="s">
+      <c r="K216" s="4" t="s">
         <v>640</v>
       </c>
       <c r="L216" t="s">
@@ -13282,8 +14042,11 @@
       <c r="O216" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P216" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>69587</v>
       </c>
@@ -13314,7 +14077,7 @@
       <c r="J217" t="s">
         <v>20</v>
       </c>
-      <c r="K217" t="s">
+      <c r="K217" s="4" t="s">
         <v>644</v>
       </c>
       <c r="L217" t="s">
@@ -13329,8 +14092,14 @@
       <c r="O217" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P217" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q217" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>69587</v>
       </c>
@@ -13361,7 +14130,7 @@
       <c r="J218" t="s">
         <v>20</v>
       </c>
-      <c r="K218" t="s">
+      <c r="K218" s="4" t="s">
         <v>645</v>
       </c>
       <c r="L218" t="s">
@@ -13376,15 +14145,18 @@
       <c r="O218" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P218" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>65831</v>
       </c>
       <c r="B219" t="s">
         <v>646</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="4" t="s">
         <v>647</v>
       </c>
       <c r="D219" t="s">
@@ -13408,7 +14180,7 @@
       <c r="J219" t="s">
         <v>20</v>
       </c>
-      <c r="K219" t="s">
+      <c r="K219" s="4" t="s">
         <v>647</v>
       </c>
       <c r="L219" t="s">
@@ -13423,8 +14195,11 @@
       <c r="O219" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P219" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>114329</v>
       </c>
@@ -13455,7 +14230,7 @@
       <c r="J220" t="s">
         <v>20</v>
       </c>
-      <c r="K220" t="s">
+      <c r="K220" s="4" t="s">
         <v>649</v>
       </c>
       <c r="L220" t="s">
@@ -13470,8 +14245,11 @@
       <c r="O220" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P220" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>114328</v>
       </c>
@@ -13517,8 +14295,11 @@
       <c r="O221" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P221" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>113975</v>
       </c>
@@ -13549,7 +14330,7 @@
       <c r="J222" t="s">
         <v>20</v>
       </c>
-      <c r="K222" t="s">
+      <c r="K222" s="4" t="s">
         <v>652</v>
       </c>
       <c r="L222" t="s">
@@ -13564,8 +14345,11 @@
       <c r="O222" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P222" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>113495</v>
       </c>
@@ -13596,7 +14380,7 @@
       <c r="J223" t="s">
         <v>20</v>
       </c>
-      <c r="K223" t="s">
+      <c r="K223" s="4" t="s">
         <v>654</v>
       </c>
       <c r="L223" t="s">
@@ -13611,8 +14395,11 @@
       <c r="O223" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P223" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>113200</v>
       </c>
@@ -13643,7 +14430,7 @@
       <c r="J224" t="s">
         <v>20</v>
       </c>
-      <c r="K224" t="s">
+      <c r="K224" s="4" t="s">
         <v>657</v>
       </c>
       <c r="L224" t="s">
@@ -13658,8 +14445,11 @@
       <c r="O224" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P224" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>112331</v>
       </c>
@@ -13690,7 +14480,7 @@
       <c r="J225" t="s">
         <v>20</v>
       </c>
-      <c r="K225" t="s">
+      <c r="K225" s="4" t="s">
         <v>659</v>
       </c>
       <c r="L225" t="s">
@@ -13705,8 +14495,11 @@
       <c r="O225" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P225" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>110170</v>
       </c>
@@ -13737,7 +14530,7 @@
       <c r="J226" t="s">
         <v>20</v>
       </c>
-      <c r="K226" t="s">
+      <c r="K226" s="4" t="s">
         <v>661</v>
       </c>
       <c r="L226" t="s">
@@ -13752,8 +14545,11 @@
       <c r="O226" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P226" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>109468</v>
       </c>
@@ -13784,7 +14580,7 @@
       <c r="J227" t="s">
         <v>20</v>
       </c>
-      <c r="K227" t="s">
+      <c r="K227" s="4" t="s">
         <v>663</v>
       </c>
       <c r="L227" t="s">
@@ -13799,8 +14595,11 @@
       <c r="O227" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P227" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>108255</v>
       </c>
@@ -13831,7 +14630,7 @@
       <c r="J228" t="s">
         <v>20</v>
       </c>
-      <c r="K228" t="s">
+      <c r="K228" s="4" t="s">
         <v>664</v>
       </c>
       <c r="L228" t="s">
@@ -13846,8 +14645,11 @@
       <c r="O228" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P228" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>106838</v>
       </c>
@@ -13878,7 +14680,7 @@
       <c r="J229" t="s">
         <v>20</v>
       </c>
-      <c r="K229" t="s">
+      <c r="K229" s="4" t="s">
         <v>666</v>
       </c>
       <c r="L229" t="s">
@@ -13893,8 +14695,11 @@
       <c r="O229" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P229" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>106838</v>
       </c>
@@ -13925,7 +14730,7 @@
       <c r="J230" t="s">
         <v>20</v>
       </c>
-      <c r="K230" t="s">
+      <c r="K230" s="4" t="s">
         <v>666</v>
       </c>
       <c r="L230" t="s">
@@ -13940,8 +14745,11 @@
       <c r="O230" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P230" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>105752</v>
       </c>
@@ -13987,8 +14795,11 @@
       <c r="O231" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P231" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>105752</v>
       </c>
@@ -14019,7 +14830,7 @@
       <c r="J232" t="s">
         <v>20</v>
       </c>
-      <c r="K232" t="s">
+      <c r="K232" s="4" t="s">
         <v>667</v>
       </c>
       <c r="L232" t="s">
@@ -14034,8 +14845,11 @@
       <c r="O232" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P232" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>105028</v>
       </c>
@@ -14080,6 +14894,9 @@
       </c>
       <c r="O233" t="s">
         <v>634</v>
+      </c>
+      <c r="P233" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -14132,8 +14949,196 @@
     <hyperlink ref="K49" r:id="rId46"/>
     <hyperlink ref="K50" r:id="rId47"/>
     <hyperlink ref="K51" r:id="rId48"/>
+    <hyperlink ref="K52" r:id="rId49"/>
+    <hyperlink ref="K53" r:id="rId50"/>
+    <hyperlink ref="K54" r:id="rId51"/>
+    <hyperlink ref="R54" r:id="rId52"/>
+    <hyperlink ref="K55" r:id="rId53"/>
+    <hyperlink ref="K56" r:id="rId54"/>
+    <hyperlink ref="K57" r:id="rId55"/>
+    <hyperlink ref="K58" r:id="rId56"/>
+    <hyperlink ref="K59" r:id="rId57"/>
+    <hyperlink ref="K60" r:id="rId58"/>
+    <hyperlink ref="K61" r:id="rId59"/>
+    <hyperlink ref="K62" r:id="rId60"/>
+    <hyperlink ref="K63" r:id="rId61"/>
+    <hyperlink ref="K64" r:id="rId62"/>
+    <hyperlink ref="K65" r:id="rId63"/>
+    <hyperlink ref="K66" r:id="rId64"/>
+    <hyperlink ref="K67" r:id="rId65"/>
+    <hyperlink ref="K68" r:id="rId66"/>
+    <hyperlink ref="K69" r:id="rId67"/>
+    <hyperlink ref="K70" r:id="rId68"/>
+    <hyperlink ref="K71" r:id="rId69"/>
+    <hyperlink ref="K72" r:id="rId70"/>
+    <hyperlink ref="K73" r:id="rId71"/>
+    <hyperlink ref="K74" r:id="rId72"/>
+    <hyperlink ref="K75" r:id="rId73"/>
+    <hyperlink ref="K76" r:id="rId74"/>
+    <hyperlink ref="K77" r:id="rId75"/>
+    <hyperlink ref="K78" r:id="rId76"/>
+    <hyperlink ref="K79" r:id="rId77"/>
+    <hyperlink ref="K80" r:id="rId78"/>
+    <hyperlink ref="K81" r:id="rId79"/>
+    <hyperlink ref="K82" r:id="rId80"/>
+    <hyperlink ref="K83" r:id="rId81"/>
+    <hyperlink ref="K84" r:id="rId82"/>
+    <hyperlink ref="K85" r:id="rId83"/>
+    <hyperlink ref="K86" r:id="rId84"/>
+    <hyperlink ref="K87" r:id="rId85"/>
+    <hyperlink ref="K88" r:id="rId86"/>
+    <hyperlink ref="K89" r:id="rId87"/>
+    <hyperlink ref="K90" r:id="rId88"/>
+    <hyperlink ref="K91" r:id="rId89"/>
+    <hyperlink ref="K92" r:id="rId90"/>
+    <hyperlink ref="K93" r:id="rId91"/>
+    <hyperlink ref="K94" r:id="rId92"/>
+    <hyperlink ref="K95" r:id="rId93"/>
+    <hyperlink ref="K96" r:id="rId94"/>
+    <hyperlink ref="K97" r:id="rId95"/>
+    <hyperlink ref="K98" r:id="rId96"/>
+    <hyperlink ref="K99" r:id="rId97"/>
+    <hyperlink ref="K100" r:id="rId98"/>
+    <hyperlink ref="K101" r:id="rId99"/>
+    <hyperlink ref="K102" r:id="rId100"/>
+    <hyperlink ref="K103" r:id="rId101"/>
+    <hyperlink ref="K104" r:id="rId102"/>
+    <hyperlink ref="K105" r:id="rId103"/>
+    <hyperlink ref="K106" r:id="rId104"/>
+    <hyperlink ref="K107" r:id="rId105"/>
+    <hyperlink ref="K108" r:id="rId106"/>
+    <hyperlink ref="K109" r:id="rId107"/>
+    <hyperlink ref="K110" r:id="rId108"/>
+    <hyperlink ref="K111" r:id="rId109"/>
+    <hyperlink ref="K112" r:id="rId110" location="mission=OCO-2"/>
+    <hyperlink ref="K113" r:id="rId111"/>
+    <hyperlink ref="K114" r:id="rId112"/>
+    <hyperlink ref="K115" r:id="rId113"/>
+    <hyperlink ref="K116" r:id="rId114"/>
+    <hyperlink ref="K117" r:id="rId115"/>
+    <hyperlink ref="K118" r:id="rId116"/>
+    <hyperlink ref="K119" r:id="rId117"/>
+    <hyperlink ref="K120" r:id="rId118"/>
+    <hyperlink ref="K121" r:id="rId119" location="mission=OCOâ€2"/>
+    <hyperlink ref="R121" r:id="rId120" location="mission=OCO-2"/>
+    <hyperlink ref="K122" r:id="rId121"/>
+    <hyperlink ref="K123" r:id="rId122"/>
+    <hyperlink ref="R123" r:id="rId123"/>
+    <hyperlink ref="K124" r:id="rId124"/>
+    <hyperlink ref="K125" r:id="rId125"/>
+    <hyperlink ref="K126" r:id="rId126"/>
+    <hyperlink ref="K127" r:id="rId127"/>
+    <hyperlink ref="K128" r:id="rId128"/>
+    <hyperlink ref="K129" r:id="rId129"/>
+    <hyperlink ref="K130" r:id="rId130"/>
+    <hyperlink ref="K131" r:id="rId131"/>
+    <hyperlink ref="K132" r:id="rId132"/>
+    <hyperlink ref="K133" r:id="rId133"/>
+    <hyperlink ref="K134" r:id="rId134"/>
+    <hyperlink ref="K135" r:id="rId135"/>
+    <hyperlink ref="K136" r:id="rId136"/>
+    <hyperlink ref="K137" r:id="rId137"/>
+    <hyperlink ref="K138" r:id="rId138"/>
+    <hyperlink ref="K139" r:id="rId139"/>
+    <hyperlink ref="K140" r:id="rId140"/>
+    <hyperlink ref="K141" r:id="rId141"/>
+    <hyperlink ref="K142" r:id="rId142"/>
+    <hyperlink ref="K143" r:id="rId143"/>
+    <hyperlink ref="K144" r:id="rId144"/>
+    <hyperlink ref="K145" r:id="rId145"/>
+    <hyperlink ref="K146" r:id="rId146"/>
+    <hyperlink ref="K147" r:id="rId147"/>
+    <hyperlink ref="K148" r:id="rId148"/>
+    <hyperlink ref="K149" r:id="rId149"/>
+    <hyperlink ref="K150" r:id="rId150"/>
+    <hyperlink ref="K151" r:id="rId151"/>
+    <hyperlink ref="K152" r:id="rId152"/>
+    <hyperlink ref="K153" r:id="rId153"/>
+    <hyperlink ref="R153" r:id="rId154"/>
+    <hyperlink ref="K154" r:id="rId155"/>
+    <hyperlink ref="K155" r:id="rId156"/>
+    <hyperlink ref="R155" r:id="rId157"/>
+    <hyperlink ref="K156" r:id="rId158"/>
+    <hyperlink ref="K157" r:id="rId159"/>
+    <hyperlink ref="K158" r:id="rId160"/>
+    <hyperlink ref="K159" r:id="rId161"/>
+    <hyperlink ref="K160" r:id="rId162"/>
+    <hyperlink ref="K161" r:id="rId163"/>
+    <hyperlink ref="K162" r:id="rId164"/>
+    <hyperlink ref="K163" r:id="rId165"/>
+    <hyperlink ref="K164" r:id="rId166"/>
+    <hyperlink ref="K165" r:id="rId167"/>
+    <hyperlink ref="K166" r:id="rId168"/>
+    <hyperlink ref="K167" r:id="rId169"/>
+    <hyperlink ref="C167" r:id="rId170"/>
+    <hyperlink ref="K168" r:id="rId171"/>
+    <hyperlink ref="K169" r:id="rId172"/>
+    <hyperlink ref="K170" r:id="rId173"/>
+    <hyperlink ref="K171" r:id="rId174"/>
+    <hyperlink ref="K172" r:id="rId175"/>
+    <hyperlink ref="K173" r:id="rId176"/>
+    <hyperlink ref="K174" r:id="rId177"/>
+    <hyperlink ref="K175" r:id="rId178"/>
+    <hyperlink ref="K176" r:id="rId179"/>
+    <hyperlink ref="K177" r:id="rId180"/>
+    <hyperlink ref="K178" r:id="rId181"/>
+    <hyperlink ref="K179" r:id="rId182"/>
+    <hyperlink ref="K180" r:id="rId183"/>
+    <hyperlink ref="K181" r:id="rId184"/>
+    <hyperlink ref="K182" r:id="rId185"/>
+    <hyperlink ref="K183" r:id="rId186"/>
+    <hyperlink ref="K184" r:id="rId187"/>
+    <hyperlink ref="K185" r:id="rId188"/>
+    <hyperlink ref="K186" r:id="rId189"/>
+    <hyperlink ref="K187" r:id="rId190"/>
+    <hyperlink ref="K188" r:id="rId191"/>
+    <hyperlink ref="K189" r:id="rId192"/>
+    <hyperlink ref="K190" r:id="rId193"/>
+    <hyperlink ref="K191" r:id="rId194"/>
+    <hyperlink ref="K192" r:id="rId195"/>
+    <hyperlink ref="K193" r:id="rId196"/>
+    <hyperlink ref="K194" r:id="rId197"/>
+    <hyperlink ref="K195" r:id="rId198"/>
+    <hyperlink ref="K196" r:id="rId199"/>
+    <hyperlink ref="K197" r:id="rId200"/>
+    <hyperlink ref="K198" r:id="rId201"/>
+    <hyperlink ref="K199" r:id="rId202"/>
+    <hyperlink ref="K200" r:id="rId203"/>
+    <hyperlink ref="K201" r:id="rId204"/>
+    <hyperlink ref="K202" r:id="rId205"/>
+    <hyperlink ref="K203" r:id="rId206"/>
+    <hyperlink ref="K204" r:id="rId207"/>
+    <hyperlink ref="K205" r:id="rId208"/>
+    <hyperlink ref="K206" r:id="rId209"/>
+    <hyperlink ref="K207" r:id="rId210"/>
+    <hyperlink ref="K208" r:id="rId211"/>
+    <hyperlink ref="K209" r:id="rId212"/>
+    <hyperlink ref="K210" r:id="rId213"/>
+    <hyperlink ref="K211" r:id="rId214"/>
+    <hyperlink ref="K212" r:id="rId215"/>
+    <hyperlink ref="K213" r:id="rId216"/>
+    <hyperlink ref="C213" r:id="rId217"/>
+    <hyperlink ref="C216" r:id="rId218"/>
+    <hyperlink ref="C219" r:id="rId219"/>
+    <hyperlink ref="K214" r:id="rId220"/>
+    <hyperlink ref="K215" r:id="rId221"/>
+    <hyperlink ref="K216" r:id="rId222"/>
+    <hyperlink ref="K217" r:id="rId223"/>
+    <hyperlink ref="K218" r:id="rId224"/>
+    <hyperlink ref="K219" r:id="rId225"/>
+    <hyperlink ref="K220" r:id="rId226"/>
+    <hyperlink ref="K222" r:id="rId227"/>
+    <hyperlink ref="K224" r:id="rId228"/>
+    <hyperlink ref="K223" r:id="rId229"/>
+    <hyperlink ref="K225" r:id="rId230"/>
+    <hyperlink ref="K226" r:id="rId231"/>
+    <hyperlink ref="K227" r:id="rId232"/>
+    <hyperlink ref="K228" r:id="rId233"/>
+    <hyperlink ref="K229" r:id="rId234"/>
+    <hyperlink ref="K230" r:id="rId235"/>
+    <hyperlink ref="K232" r:id="rId236"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId49"/>
+  <pageSetup orientation="portrait" r:id="rId237"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated figures in analysis
</commit_message>
<xml_diff>
--- a/analysis_2023-05/linksToCheck.xlsx
+++ b/analysis_2023-05/linksToCheck.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22092" windowHeight="7860" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22092" windowHeight="7860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="4-linksToCheck" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,13 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="716">
   <si>
     <t>eprint_id</t>
   </si>
@@ -2169,6 +2169,12 @@
   </si>
   <si>
     <t>(Multiple Items)</t>
+  </si>
+  <si>
+    <t>All URL</t>
+  </si>
+  <si>
+    <t>Rest</t>
   </si>
 </sst>
 </file>
@@ -2750,7 +2756,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Older Datasets</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> are More Likely to be Missing</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.1597112860892389E-2"/>
+          <c:y val="4.1666666666666664E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2907,11 +2950,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Year!$T$4:$T$26</c15:sqref>
+                    <c15:sqref>Year!$W$4:$W$26</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Year!$T$5:$T$13</c:f>
+              <c:f>Year!$W$5:$W$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2971,8 +3014,69 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Year of Article</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Publication</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -3020,53 +3124,77 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent of Links that Fail</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="350578640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -3663,13 +3791,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>556260</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -8610,7 +8738,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:P10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -8745,7 +8873,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:K21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -8927,7 +9055,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -9062,7 +9190,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B75" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -9476,7 +9604,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -21862,10 +21990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P10"/>
+  <dimension ref="A3:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21888,7 +22016,7 @@
     <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>706</v>
       </c>
@@ -21896,7 +22024,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>701</v>
       </c>
@@ -21945,8 +22073,21 @@
       <c r="P4" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R4" t="s">
+        <v>634</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4">
+        <v>21</v>
+      </c>
+      <c r="U4">
+        <f>S4/T4</f>
+        <v>0.23809523809523808</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>686</v>
       </c>
@@ -21969,8 +22110,21 @@
       <c r="P5" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>414</v>
+      </c>
+      <c r="S5">
+        <v>13</v>
+      </c>
+      <c r="T5">
+        <v>744</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U6" si="0">S5/T5</f>
+        <v>1.7473118279569891E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>678</v>
       </c>
@@ -21995,8 +22149,21 @@
       <c r="P6" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R6" t="s">
+        <v>714</v>
+      </c>
+      <c r="S6">
+        <v>100</v>
+      </c>
+      <c r="T6">
+        <v>1401</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>7.1377587437544618E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>702</v>
       </c>
@@ -22036,7 +22203,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>703</v>
       </c>
@@ -22082,7 +22249,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>704</v>
       </c>
@@ -22102,7 +22269,7 @@
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>705</v>
       </c>
@@ -22157,10 +22324,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView topLeftCell="G3" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="O4" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5:T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22181,12 +22348,12 @@
     <col min="14" max="14" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="8"/>
+    <col min="17" max="20" width="8.88671875" customWidth="1"/>
+    <col min="22" max="22" width="8.88671875" customWidth="1"/>
+    <col min="23" max="23" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>670</v>
       </c>
@@ -22194,15 +22361,24 @@
         <v>702</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>709</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R3" t="s">
+        <v>414</v>
+      </c>
+      <c r="S3" t="s">
+        <v>634</v>
+      </c>
+      <c r="T3" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>701</v>
       </c>
@@ -22239,15 +22415,18 @@
       <c r="Q4" s="6">
         <v>2023</v>
       </c>
-      <c r="S4" s="7">
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="V4" s="7">
         <v>4</v>
       </c>
-      <c r="T4" s="8">
-        <f>R4/S4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="W4" s="8">
+        <f t="shared" ref="W4:W23" si="0">U4/V4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2004</v>
       </c>
@@ -22268,18 +22447,26 @@
       <c r="Q5" s="6">
         <v>2022</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="6"/>
+      <c r="S5" s="6">
+        <v>2</v>
+      </c>
+      <c r="T5" s="6">
+        <f>U5-S5-R5</f>
+        <v>6</v>
+      </c>
+      <c r="U5" s="7">
         <v>8</v>
       </c>
-      <c r="S5" s="7">
+      <c r="V5" s="7">
         <v>619</v>
       </c>
-      <c r="T5" s="8">
-        <f>R5/S5</f>
+      <c r="W5" s="8">
+        <f t="shared" si="0"/>
         <v>1.2924071082390954E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2006</v>
       </c>
@@ -22300,18 +22487,28 @@
       <c r="Q6" s="6">
         <v>2021</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="6">
+        <v>5</v>
+      </c>
+      <c r="S6" s="6">
+        <v>1</v>
+      </c>
+      <c r="T6" s="6">
+        <f t="shared" ref="T6:T26" si="1">U6-S6-R6</f>
+        <v>25</v>
+      </c>
+      <c r="U6" s="7">
         <v>31</v>
       </c>
-      <c r="S6" s="7">
+      <c r="V6" s="7">
         <v>747</v>
       </c>
-      <c r="T6" s="8">
-        <f>R6/S6</f>
+      <c r="W6" s="8">
+        <f t="shared" si="0"/>
         <v>4.1499330655957165E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>2007</v>
       </c>
@@ -22332,18 +22529,28 @@
       <c r="Q7" s="6">
         <v>2020</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="6">
+        <v>6</v>
+      </c>
+      <c r="S7" s="6">
+        <v>2</v>
+      </c>
+      <c r="T7" s="6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="U7" s="7">
         <v>23</v>
       </c>
-      <c r="S7" s="7">
+      <c r="V7" s="7">
         <v>383</v>
       </c>
-      <c r="T7" s="8">
-        <f>R7/S7</f>
+      <c r="W7" s="8">
+        <f t="shared" si="0"/>
         <v>6.0052219321148827E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2009</v>
       </c>
@@ -22364,18 +22571,26 @@
       <c r="Q8" s="6">
         <v>2019</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="6">
+        <v>1</v>
+      </c>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U8" s="7">
         <v>5</v>
       </c>
-      <c r="S8" s="7">
+      <c r="V8" s="7">
         <v>114</v>
       </c>
-      <c r="T8" s="8">
-        <f>R8/S8</f>
+      <c r="W8" s="8">
+        <f t="shared" si="0"/>
         <v>4.3859649122807015E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>2010</v>
       </c>
@@ -22398,18 +22613,24 @@
       <c r="Q9" s="6">
         <v>2018</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="S9" s="7">
+      <c r="U9" s="7">
+        <v>5</v>
+      </c>
+      <c r="V9" s="7">
         <v>51</v>
       </c>
-      <c r="T9" s="8">
-        <f>R9/S9</f>
+      <c r="W9" s="8">
+        <f t="shared" si="0"/>
         <v>9.8039215686274508E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>2012</v>
       </c>
@@ -22430,18 +22651,24 @@
       <c r="Q10" s="6">
         <v>2017</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="S10" s="7">
+      <c r="U10" s="7">
+        <v>5</v>
+      </c>
+      <c r="V10" s="7">
         <v>24</v>
       </c>
-      <c r="T10" s="8">
-        <f>R10/S10</f>
+      <c r="W10" s="8">
+        <f t="shared" si="0"/>
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>2013</v>
       </c>
@@ -22462,18 +22689,26 @@
       <c r="Q11" s="6">
         <v>2016</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="6">
+        <v>1</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="U11" s="7">
         <v>10</v>
       </c>
-      <c r="S11" s="7">
+      <c r="V11" s="7">
         <v>57</v>
       </c>
-      <c r="T11" s="8">
-        <f>R11/S11</f>
+      <c r="W11" s="8">
+        <f t="shared" si="0"/>
         <v>0.17543859649122806</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>2014</v>
       </c>
@@ -22496,18 +22731,24 @@
       <c r="Q12" s="6">
         <v>2015</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="S12" s="7">
+      <c r="U12" s="7">
+        <v>6</v>
+      </c>
+      <c r="V12" s="7">
         <v>53</v>
       </c>
-      <c r="T12" s="8">
-        <f>R12/S12</f>
+      <c r="W12" s="8">
+        <f t="shared" si="0"/>
         <v>0.11320754716981132</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>2015</v>
       </c>
@@ -22532,18 +22773,24 @@
       <c r="Q13" s="6">
         <v>2014</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="S13" s="7">
+      <c r="U13" s="7">
+        <v>12</v>
+      </c>
+      <c r="V13" s="7">
         <v>43</v>
       </c>
-      <c r="T13" s="8">
-        <f>R13/S13</f>
+      <c r="W13" s="8">
+        <f t="shared" si="0"/>
         <v>0.27906976744186046</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>2016</v>
       </c>
@@ -22570,18 +22817,24 @@
       <c r="Q14" s="6">
         <v>2013</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="S14" s="7">
+      <c r="U14" s="7">
+        <v>2</v>
+      </c>
+      <c r="V14" s="7">
         <v>5</v>
       </c>
-      <c r="T14" s="8">
-        <f>R14/S14</f>
+      <c r="W14" s="8">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>2017</v>
       </c>
@@ -22604,18 +22857,24 @@
       <c r="Q15" s="6">
         <v>2012</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="S15" s="7">
+      <c r="U15" s="7">
+        <v>1</v>
+      </c>
+      <c r="V15" s="7">
         <v>6</v>
       </c>
-      <c r="T15" s="8">
-        <f>R15/S15</f>
+      <c r="W15" s="8">
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>2018</v>
       </c>
@@ -22638,15 +22897,21 @@
       <c r="Q16" s="6">
         <v>2011</v>
       </c>
-      <c r="S16" s="7">
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="7">
         <v>3</v>
       </c>
-      <c r="T16" s="8">
-        <f>R16/S16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="W16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>2019</v>
       </c>
@@ -22671,18 +22936,24 @@
       <c r="Q17" s="6">
         <v>2010</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="S17" s="7">
+      <c r="U17" s="7">
+        <v>2</v>
+      </c>
+      <c r="V17" s="7">
         <v>3</v>
       </c>
-      <c r="T17" s="8">
-        <f>R17/S17</f>
+      <c r="W17" s="8">
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>2020</v>
       </c>
@@ -22709,18 +22980,24 @@
       <c r="Q18" s="6">
         <v>2009</v>
       </c>
-      <c r="R18" s="7">
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="S18" s="7">
+      <c r="U18" s="7">
+        <v>1</v>
+      </c>
+      <c r="V18" s="7">
         <v>2</v>
       </c>
-      <c r="T18" s="8">
-        <f>R18/S18</f>
+      <c r="W18" s="8">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>2021</v>
       </c>
@@ -22747,15 +23024,21 @@
       <c r="Q19" s="6">
         <v>2008</v>
       </c>
-      <c r="S19" s="7">
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="7">
         <v>10</v>
       </c>
-      <c r="T19" s="8">
-        <f>R19/S19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="W19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>2022</v>
       </c>
@@ -22778,18 +23061,24 @@
       <c r="Q20" s="6">
         <v>2007</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="S20" s="7">
+      <c r="U20" s="7">
+        <v>2</v>
+      </c>
+      <c r="V20" s="7">
         <v>7</v>
       </c>
-      <c r="T20" s="8">
-        <f>R20/S20</f>
+      <c r="W20" s="8">
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>705</v>
       </c>
@@ -22826,87 +23115,123 @@
       <c r="Q21" s="6">
         <v>2006</v>
       </c>
-      <c r="R21" s="7">
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="S21" s="7">
+      <c r="U21" s="7">
+        <v>2</v>
+      </c>
+      <c r="V21" s="7">
         <v>7</v>
       </c>
-      <c r="T21" s="8">
-        <f>R21/S21</f>
+      <c r="W21" s="8">
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q22" s="6">
         <v>2005</v>
       </c>
-      <c r="S22" s="7">
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="7">
         <v>3</v>
       </c>
-      <c r="T22" s="8">
-        <f>R22/S22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="W22" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q23" s="6">
         <v>2004</v>
       </c>
-      <c r="R23" s="7">
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="S23" s="7">
+      <c r="U23" s="7">
+        <v>3</v>
+      </c>
+      <c r="V23" s="7">
         <v>9</v>
       </c>
-      <c r="T23" s="8">
-        <f>R23/S23</f>
+      <c r="W23" s="8">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q24" s="6">
         <v>2003</v>
       </c>
-      <c r="S24" s="7">
-        <v>0</v>
-      </c>
-      <c r="T24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="7">
+        <v>0</v>
+      </c>
+      <c r="W24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q25" s="6">
         <v>2002</v>
       </c>
-      <c r="S25" s="7">
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V25" s="7">
         <v>4</v>
       </c>
-      <c r="T25" s="8">
-        <f>R25/S25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="W25" s="8">
+        <f>U25/V25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q26" s="6">
         <v>2001</v>
       </c>
-      <c r="S26" s="7">
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="7">
         <v>8</v>
       </c>
-      <c r="T26" s="8">
-        <f>R26/S26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="T27"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="T28"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="T29"/>
+      <c r="W26" s="8">
+        <f>U26/V26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W27"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W28"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22990,7 +23315,7 @@
         <v>1342</v>
       </c>
       <c r="M5" s="8">
-        <f>K5/L5</f>
+        <f t="shared" ref="M5:M17" si="0">K5/L5</f>
         <v>5.8867362146050671E-2</v>
       </c>
     </row>
@@ -23020,7 +23345,7 @@
         <v>744</v>
       </c>
       <c r="M6" s="8">
-        <f>K6/L6</f>
+        <f t="shared" si="0"/>
         <v>1.7473118279569891E-2</v>
       </c>
     </row>
@@ -23050,7 +23375,7 @@
         <v>21</v>
       </c>
       <c r="M7" s="8">
-        <f>K7/L7</f>
+        <f t="shared" si="0"/>
         <v>0.23809523809523808</v>
       </c>
     </row>
@@ -23082,7 +23407,7 @@
         <v>16</v>
       </c>
       <c r="M8" s="8">
-        <f>K8/L8</f>
+        <f t="shared" si="0"/>
         <v>0.4375</v>
       </c>
     </row>
@@ -23112,7 +23437,7 @@
         <v>12</v>
       </c>
       <c r="M9" s="8">
-        <f>K9/L9</f>
+        <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
     </row>
@@ -23142,7 +23467,7 @@
         <v>9</v>
       </c>
       <c r="M10" s="8">
-        <f>K10/L10</f>
+        <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
     </row>
@@ -23170,7 +23495,7 @@
         <v>7</v>
       </c>
       <c r="M11" s="8">
-        <f>K11/L11</f>
+        <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -23198,7 +23523,7 @@
         <v>5</v>
       </c>
       <c r="M12" s="8">
-        <f>K12/L12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -23226,7 +23551,7 @@
         <v>3</v>
       </c>
       <c r="M13" s="8">
-        <f>K13/L13</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -23258,7 +23583,7 @@
         <v>3</v>
       </c>
       <c r="M14" s="8">
-        <f>K14/L14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -23284,7 +23609,7 @@
         <v>2</v>
       </c>
       <c r="M15" s="8">
-        <f>K15/L15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -23312,7 +23637,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="8">
-        <f>K16/L16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -23340,7 +23665,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="8">
-        <f>K17/L17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -23388,7 +23713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added fit link to figure 2
</commit_message>
<xml_diff>
--- a/analysis_2023-05/linksToCheck.xlsx
+++ b/analysis_2023-05/linksToCheck.xlsx
@@ -2902,6 +2902,54 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.42075524934383202"/>
+                  <c:y val="0.14907042869641296"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:extLst>
@@ -10007,7 +10055,7 @@
   <dimension ref="A1:R233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:R1048576"/>
     </sheetView>
   </sheetViews>
@@ -22326,8 +22374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O4" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5:T26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4:U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23245,7 +23293,7 @@
   <dimension ref="A3:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:M7"/>
+      <selection activeCell="J5" sqref="J5:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23713,8 +23761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>